<commit_message>
Added data on BC_Country, but not done yet
</commit_message>
<xml_diff>
--- a/Oracle/Assignment 4/IS-309 FINAL EXCEL.xlsx
+++ b/Oracle/Assignment 4/IS-309 FINAL EXCEL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03723F51-6BD2-F74F-9CAD-7CDF0CC089FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A539AA-403D-A44A-8797-E9A4E0A7C3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="19200" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uprise Art" sheetId="2" r:id="rId1"/>
@@ -347,7 +347,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,6 +401,7 @@
     <xf numFmtId="10" fontId="0" fillId="9" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -752,10 +753,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1056,8 +1057,12 @@
       <c r="E5" s="35">
         <v>0</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="F5" s="37">
+        <v>249</v>
+      </c>
+      <c r="G5" s="39">
+        <v>0</v>
+      </c>
       <c r="H5" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1067,11 +1072,11 @@
       </c>
       <c r="J5" s="23">
         <f>B5*F5*(1+E5/100)*(1+I5/100)</f>
-        <v>0</v>
+        <v>6225</v>
       </c>
       <c r="K5" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.0791015625</v>
       </c>
       <c r="L5" s="20">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
Pushed up the contributions and some tweaking on the sheet and .sql file
</commit_message>
<xml_diff>
--- a/Oracle/Assignment 4/IS-309 FINAL EXCEL.xlsx
+++ b/Oracle/Assignment 4/IS-309 FINAL EXCEL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D7BAAA-CE7B-BD48-858F-F4CE5DA69EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4592A42-3D48-4F4A-8DDA-3C78F1883F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="11740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uprise Art" sheetId="2" r:id="rId1"/>
@@ -743,10 +743,10 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="161" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,7 +894,7 @@
         <v>983040</v>
       </c>
       <c r="R2" s="28">
-        <f>Q2/1024</f>
+        <f t="shared" ref="R2:R11" si="0">Q2/1024</f>
         <v>960</v>
       </c>
       <c r="S2" s="28" t="s">
@@ -927,18 +927,18 @@
         <v>2500</v>
       </c>
       <c r="H3" s="15">
-        <f t="shared" ref="H3:H11" si="0">G3/2</f>
+        <f t="shared" ref="H3:H11" si="1">G3/2</f>
         <v>1250</v>
       </c>
       <c r="I3" s="22">
         <v>0</v>
       </c>
       <c r="J3" s="16">
-        <f t="shared" ref="J3:J11" si="1">B3*F3*(1+E3/100)*(1+I3/100)</f>
+        <f t="shared" ref="J3:J11" si="2">B3*F3*(1+E3/100)*(1+I3/100)</f>
         <v>12636000</v>
       </c>
       <c r="K3" s="18">
-        <f t="shared" ref="K3:K11" si="2">J3/1024</f>
+        <f t="shared" ref="K3:K11" si="3">J3/1024</f>
         <v>12339.84375</v>
       </c>
       <c r="L3" s="19">
@@ -946,11 +946,11 @@
         <v>97500</v>
       </c>
       <c r="M3" s="15">
-        <f t="shared" ref="M3:M11" si="3">L3/1024</f>
+        <f t="shared" ref="M3:M11" si="4">L3/1024</f>
         <v>95.21484375</v>
       </c>
       <c r="N3" s="27">
-        <f t="shared" ref="N3:N11" si="4">O3*_xlfn.CEILING.MATH(K3/O3)</f>
+        <f t="shared" ref="N3:N11" si="5">O3*_xlfn.CEILING.MATH(K3/O3)</f>
         <v>12416</v>
       </c>
       <c r="O3" s="28">
@@ -958,15 +958,15 @@
         <v>128</v>
       </c>
       <c r="P3" s="28">
-        <f t="shared" ref="P3:P11" si="5">O3/1024</f>
+        <f t="shared" ref="P3:P11" si="6">O3/1024</f>
         <v>0.125</v>
       </c>
       <c r="Q3" s="28">
-        <f t="shared" ref="Q3:Q11" si="6">N3+(2*O3)</f>
+        <f t="shared" ref="Q3:Q11" si="7">N3+(2*O3)</f>
         <v>12672</v>
       </c>
       <c r="R3" s="28">
-        <f>Q3/1024</f>
+        <f t="shared" si="0"/>
         <v>12.375</v>
       </c>
       <c r="S3" s="28" t="s">
@@ -984,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="17">
-        <f t="shared" ref="D4:D11" si="7">(C4/(B4+C4))</f>
+        <f t="shared" ref="D4:D11" si="8">(C4/(B4+C4))</f>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="E4" s="14">
@@ -999,46 +999,46 @@
         <v>464000000</v>
       </c>
       <c r="H4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>232000000</v>
       </c>
       <c r="I4" s="21">
         <v>10</v>
       </c>
       <c r="J4" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29568000000.000004</v>
       </c>
       <c r="K4" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28875000.000000004</v>
       </c>
       <c r="L4" s="19">
-        <f t="shared" ref="L4:L11" si="8">B4*H4*(1+E4/100)*(1+I4/100)</f>
+        <f t="shared" ref="L4:L11" si="9">B4*H4*(1+E4/100)*(1+I4/100)</f>
         <v>10718400000</v>
       </c>
       <c r="M4" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10467187.5</v>
       </c>
       <c r="N4" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33554432</v>
       </c>
       <c r="O4" s="28">
-        <f t="shared" ref="O4:O11" si="9">IF(2^_xlfn.CEILING.MATH(LOG(M4,2),1) &lt; 64, "64", 2^_xlfn.CEILING.MATH(LOG(M4,2),1))</f>
+        <f>IF(2^_xlfn.CEILING.MATH(LOG(M4,2),1) &lt; 64, "64", 2^_xlfn.CEILING.MATH(LOG(M4,2),1))</f>
         <v>16777216</v>
       </c>
       <c r="P4" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16384</v>
       </c>
       <c r="Q4" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>67108864</v>
       </c>
       <c r="R4" s="28">
-        <f>Q4/1024</f>
+        <f t="shared" si="0"/>
         <v>65536</v>
       </c>
       <c r="S4" s="28" t="s">
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E5" s="30">
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="32">
@@ -1080,15 +1080,15 @@
         <v>6225</v>
       </c>
       <c r="K5" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0791015625</v>
       </c>
       <c r="L5" s="33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M5" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N5" s="31">
@@ -1098,15 +1098,15 @@
         <v>64</v>
       </c>
       <c r="P5" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.25E-2</v>
       </c>
       <c r="Q5" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="R5" s="28">
-        <f>Q5/1024</f>
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
       <c r="S5" s="30" t="s">
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E6" s="14">
@@ -1139,46 +1139,46 @@
         <v>4000</v>
       </c>
       <c r="H6" s="15">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <f t="shared" si="2"/>
+        <v>9590400</v>
+      </c>
+      <c r="K6" s="18">
+        <f t="shared" si="3"/>
+        <v>9365.625</v>
+      </c>
+      <c r="L6" s="19">
+        <f t="shared" si="9"/>
+        <v>74000</v>
+      </c>
+      <c r="M6" s="15">
+        <f t="shared" si="4"/>
+        <v>72.265625</v>
+      </c>
+      <c r="N6" s="27">
+        <f t="shared" si="5"/>
+        <v>9472</v>
+      </c>
+      <c r="O6" s="28">
+        <f t="shared" ref="O4:O11" si="10">IF(2^_xlfn.CEILING.MATH(LOG(M6,2),1) &lt; 64, "64", 2^_xlfn.CEILING.MATH(LOG(M6,2),1))</f>
+        <v>128</v>
+      </c>
+      <c r="P6" s="28">
+        <f t="shared" si="6"/>
+        <v>0.125</v>
+      </c>
+      <c r="Q6" s="28">
+        <f t="shared" si="7"/>
+        <v>9728</v>
+      </c>
+      <c r="R6" s="28">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="I6" s="21">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16">
-        <f t="shared" si="1"/>
-        <v>9590400</v>
-      </c>
-      <c r="K6" s="18">
-        <f t="shared" si="2"/>
-        <v>9365.625</v>
-      </c>
-      <c r="L6" s="19">
-        <f t="shared" si="8"/>
-        <v>74000</v>
-      </c>
-      <c r="M6" s="15">
-        <f t="shared" si="3"/>
-        <v>72.265625</v>
-      </c>
-      <c r="N6" s="27">
-        <f t="shared" si="4"/>
-        <v>9472</v>
-      </c>
-      <c r="O6" s="28">
-        <f t="shared" si="9"/>
-        <v>128</v>
-      </c>
-      <c r="P6" s="28">
-        <f t="shared" si="5"/>
-        <v>0.125</v>
-      </c>
-      <c r="Q6" s="28">
-        <f t="shared" si="6"/>
-        <v>9728</v>
-      </c>
-      <c r="R6" s="28">
-        <f>Q6/1024</f>
         <v>9.5</v>
       </c>
       <c r="S6" s="28" t="s">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="E7" s="14">
@@ -1211,46 +1211,46 @@
         <v>2000000</v>
       </c>
       <c r="H7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
       <c r="I7" s="21">
         <v>10</v>
       </c>
       <c r="J7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>535920000.00000006</v>
       </c>
       <c r="K7" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>523359.37500000006</v>
       </c>
       <c r="L7" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>33495000.000000004</v>
       </c>
       <c r="M7" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32709.960937500004</v>
       </c>
       <c r="N7" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>524288</v>
       </c>
       <c r="O7" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>32768</v>
       </c>
       <c r="P7" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="Q7" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>589824</v>
       </c>
       <c r="R7" s="28">
-        <f>Q7/1024</f>
+        <f t="shared" si="0"/>
         <v>576</v>
       </c>
       <c r="S7" s="28" t="s">
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E8" s="14">
@@ -1283,46 +1283,46 @@
         <v>30</v>
       </c>
       <c r="H8" s="15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
+        <f t="shared" si="2"/>
+        <v>349920</v>
+      </c>
+      <c r="K8" s="18">
+        <f t="shared" si="3"/>
+        <v>341.71875</v>
+      </c>
+      <c r="L8" s="19">
+        <f t="shared" si="9"/>
+        <v>2700</v>
+      </c>
+      <c r="M8" s="15">
+        <f t="shared" si="4"/>
+        <v>2.63671875</v>
+      </c>
+      <c r="N8" s="27">
+        <f t="shared" si="5"/>
+        <v>384</v>
+      </c>
+      <c r="O8" s="29" t="str">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="P8" s="28">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q8" s="28">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+      <c r="R8" s="28">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16">
-        <f t="shared" si="1"/>
-        <v>349920</v>
-      </c>
-      <c r="K8" s="18">
-        <f t="shared" si="2"/>
-        <v>341.71875</v>
-      </c>
-      <c r="L8" s="19">
-        <f t="shared" si="8"/>
-        <v>2700</v>
-      </c>
-      <c r="M8" s="15">
-        <f t="shared" si="3"/>
-        <v>2.63671875</v>
-      </c>
-      <c r="N8" s="27">
-        <f t="shared" si="4"/>
-        <v>384</v>
-      </c>
-      <c r="O8" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="P8" s="28">
-        <f t="shared" si="5"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q8" s="28">
-        <f t="shared" si="6"/>
-        <v>512</v>
-      </c>
-      <c r="R8" s="28">
-        <f>Q8/1024</f>
         <v>0.5</v>
       </c>
       <c r="S8" s="28" t="s">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E9" s="14">
@@ -1353,46 +1353,46 @@
         <v>10</v>
       </c>
       <c r="H9" s="15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <f t="shared" si="2"/>
+        <v>87480</v>
+      </c>
+      <c r="K9" s="18">
+        <f t="shared" si="3"/>
+        <v>85.4296875</v>
+      </c>
+      <c r="L9" s="19">
+        <f t="shared" si="9"/>
+        <v>675</v>
+      </c>
+      <c r="M9" s="15">
+        <f t="shared" si="4"/>
+        <v>0.6591796875</v>
+      </c>
+      <c r="N9" s="27">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="O9" s="29" t="str">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="P9" s="28">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q9" s="28">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+      <c r="R9" s="28">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16">
-        <f t="shared" si="1"/>
-        <v>87480</v>
-      </c>
-      <c r="K9" s="18">
-        <f t="shared" si="2"/>
-        <v>85.4296875</v>
-      </c>
-      <c r="L9" s="19">
-        <f t="shared" si="8"/>
-        <v>675</v>
-      </c>
-      <c r="M9" s="15">
-        <f t="shared" si="3"/>
-        <v>0.6591796875</v>
-      </c>
-      <c r="N9" s="27">
-        <f t="shared" si="4"/>
-        <v>128</v>
-      </c>
-      <c r="O9" s="29" t="str">
-        <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="P9" s="28">
-        <f t="shared" si="5"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q9" s="28">
-        <f t="shared" si="6"/>
-        <v>256</v>
-      </c>
-      <c r="R9" s="28">
-        <f>Q9/1024</f>
         <v>0.25</v>
       </c>
       <c r="S9" s="28" t="s">
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E10" s="14">
@@ -1425,46 +1425,46 @@
         <v>500</v>
       </c>
       <c r="H10" s="15">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" si="2"/>
+        <v>4471200</v>
+      </c>
+      <c r="K10" s="18">
+        <f t="shared" si="3"/>
+        <v>4366.40625</v>
+      </c>
+      <c r="L10" s="19">
+        <f t="shared" si="9"/>
+        <v>34500</v>
+      </c>
+      <c r="M10" s="15">
+        <f t="shared" si="4"/>
+        <v>33.69140625</v>
+      </c>
+      <c r="N10" s="27">
+        <f t="shared" si="5"/>
+        <v>4416</v>
+      </c>
+      <c r="O10" s="28">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="P10" s="28">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q10" s="28">
+        <f t="shared" si="7"/>
+        <v>4544</v>
+      </c>
+      <c r="R10" s="28">
         <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="16">
-        <f t="shared" si="1"/>
-        <v>4471200</v>
-      </c>
-      <c r="K10" s="18">
-        <f t="shared" si="2"/>
-        <v>4366.40625</v>
-      </c>
-      <c r="L10" s="19">
-        <f t="shared" si="8"/>
-        <v>34500</v>
-      </c>
-      <c r="M10" s="15">
-        <f t="shared" si="3"/>
-        <v>33.69140625</v>
-      </c>
-      <c r="N10" s="27">
-        <f t="shared" si="4"/>
-        <v>4416</v>
-      </c>
-      <c r="O10" s="28">
-        <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="P10" s="28">
-        <f t="shared" si="5"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="Q10" s="28">
-        <f t="shared" si="6"/>
-        <v>4544</v>
-      </c>
-      <c r="R10" s="28">
-        <f>Q10/1024</f>
         <v>4.4375</v>
       </c>
       <c r="S10" s="28" t="s">
@@ -1482,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.4117647058823528E-2</v>
       </c>
       <c r="E11" s="14">
@@ -1497,46 +1497,46 @@
         <v>116000000</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58000000</v>
       </c>
       <c r="I11" s="21">
         <v>10</v>
       </c>
       <c r="J11" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14907200000.000004</v>
       </c>
       <c r="K11" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14557812.500000004</v>
       </c>
       <c r="L11" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5403860000</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5277207.03125</v>
       </c>
       <c r="N11" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16777216</v>
       </c>
       <c r="O11" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8388608</v>
       </c>
       <c r="P11" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8192</v>
       </c>
       <c r="Q11" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33554432</v>
       </c>
       <c r="R11" s="28">
-        <f>Q11/1024</f>
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="S11" s="28" t="s">
@@ -1642,15 +1642,15 @@
         <v>22400</v>
       </c>
       <c r="E17" s="26">
-        <f t="shared" ref="E17:E21" si="10">IF(2^_xlfn.CEILING.MATH(LOG(D17,2),1) &lt; 64, "64", 2^_xlfn.CEILING.MATH(LOG(D17,2),1))</f>
+        <f t="shared" ref="E17:E21" si="11">IF(2^_xlfn.CEILING.MATH(LOG(D17,2),1) &lt; 64, "64", 2^_xlfn.CEILING.MATH(LOG(D17,2),1))</f>
         <v>32768</v>
       </c>
       <c r="F17" s="26">
-        <f t="shared" ref="F17:G21" si="11">E17/1024</f>
+        <f t="shared" ref="F17:G21" si="12">E17/1024</f>
         <v>32</v>
       </c>
       <c r="G17" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.125E-2</v>
       </c>
       <c r="K17" s="2"/>
@@ -1673,15 +1673,15 @@
         <v>589824</v>
       </c>
       <c r="E18" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1048576</v>
       </c>
       <c r="F18" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1024</v>
       </c>
       <c r="G18" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K18" s="2"/>
@@ -1704,15 +1704,15 @@
         <v>65536</v>
       </c>
       <c r="E19" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>65536</v>
       </c>
       <c r="F19" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
       <c r="G19" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6.25E-2</v>
       </c>
       <c r="K19" s="2"/>
@@ -1735,11 +1735,11 @@
         <v>33554432</v>
       </c>
       <c r="E20" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>33554432</v>
       </c>
       <c r="F20" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>32768</v>
       </c>
       <c r="G20" s="26">
@@ -1762,11 +1762,11 @@
         <v>67108864</v>
       </c>
       <c r="E21" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>67108864</v>
       </c>
       <c r="F21" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>65536</v>
       </c>
       <c r="G21" s="26">

</xml_diff>